<commit_message>
Added 10k thin film resistors in 0603,0805, and 1206 sizes. Added 110k 0603,0805,1206 resistors in both thick film and thin film variants.
</commit_message>
<xml_diff>
--- a/To Add v2/Resistors - Single - SMD.xlsx
+++ b/To Add v2/Resistors - Single - SMD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\To Add v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Danakil_KiCad_DB\To Add v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10DF6B7-BCAD-4DF7-8378-E50BA79D38D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11265C5E-0E05-4E1A-AB24-B81E862A1D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1032" yWindow="2628" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12410" yWindow="0" windowWidth="13400" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="267">
   <si>
     <t>Totals</t>
   </si>
@@ -765,6 +765,78 @@
   </si>
   <si>
     <t>Stocking?</t>
+  </si>
+  <si>
+    <t>ERA-3AEB103V</t>
+  </si>
+  <si>
+    <t>P10KDBCT-ND</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>Thin Film</t>
+  </si>
+  <si>
+    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/RDM0000/AOA0000C307.pdf</t>
+  </si>
+  <si>
+    <t>ERA-6AEB103V</t>
+  </si>
+  <si>
+    <t>P10KDACT-ND</t>
+  </si>
+  <si>
+    <t>ERA-8AEB103V</t>
+  </si>
+  <si>
+    <t>P10KBCCT-ND</t>
+  </si>
+  <si>
+    <t>100v</t>
+  </si>
+  <si>
+    <t>110k</t>
+  </si>
+  <si>
+    <t>ERA-3AEB114V</t>
+  </si>
+  <si>
+    <t>P110KDBCT-ND</t>
+  </si>
+  <si>
+    <t>ERA-6AEB114V</t>
+  </si>
+  <si>
+    <t>P110KDACT-ND</t>
+  </si>
+  <si>
+    <t>ERA-8AEB114V</t>
+  </si>
+  <si>
+    <t>P110KBCCT-ND</t>
+  </si>
+  <si>
+    <t>CRCW0603110KFKEA</t>
+  </si>
+  <si>
+    <t>541-110KHCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.vishay.com/docs/20035/dcrcwe3.pdf</t>
+  </si>
+  <si>
+    <t>CRCW0805110KFKEAC</t>
+  </si>
+  <si>
+    <t>541-CRCW0805110KFKEACCT-ND</t>
+  </si>
+  <si>
+    <t>CRCW1206110KFKEA</t>
+  </si>
+  <si>
+    <t>541-110KFCT-ND</t>
   </si>
 </sst>
 </file>
@@ -832,11 +904,18 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -857,8 +936,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9DBE32F-464A-4F02-8A61-DC37E24DCD04}" name="Table1" displayName="Table1" ref="C6:S93" totalsRowShown="0">
-  <autoFilter ref="C6:S93" xr:uid="{D9DBE32F-464A-4F02-8A61-DC37E24DCD04}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9DBE32F-464A-4F02-8A61-DC37E24DCD04}" name="Table1" displayName="Table1" ref="C6:S102" totalsRowShown="0">
+  <autoFilter ref="C6:S102" xr:uid="{D9DBE32F-464A-4F02-8A61-DC37E24DCD04}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C7:S93">
     <sortCondition ref="S6:S93"/>
   </sortState>
@@ -868,7 +947,7 @@
     </tableColumn>
     <tableColumn id="2" xr3:uid="{B5BE2BAF-C919-4E34-BDBB-91FA482CB3EE}" name="Value"/>
     <tableColumn id="3" xr3:uid="{D5D09B72-E8BC-4CEE-A159-8B081CDABB64}" name="Tolerance"/>
-    <tableColumn id="4" xr3:uid="{58A7E2F1-6A01-44B9-A5AA-27E62CCC0041}" name="Size" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{58A7E2F1-6A01-44B9-A5AA-27E62CCC0041}" name="Size" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{FE7A1284-C7E7-4581-98AD-73796FB7DB6B}" name="Power"/>
     <tableColumn id="6" xr3:uid="{D30D7C30-427B-494A-AE28-B60D62B8A67E}" name="Voltage"/>
     <tableColumn id="7" xr3:uid="{34BA0C50-826E-4F58-A897-0945BFA093D2}" name="Technology"/>
@@ -1150,120 +1229,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA93"/>
+  <dimension ref="A1:AA102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S84" sqref="S84"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="2"/>
-    <col min="8" max="8" width="9.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.88671875" customWidth="1"/>
-    <col min="14" max="14" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
-    <col min="17" max="17" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" customWidth="1"/>
+    <col min="6" max="6" width="8.90625" style="2"/>
+    <col min="8" max="8" width="9.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" customWidth="1"/>
+    <col min="10" max="10" width="10.36328125" customWidth="1"/>
+    <col min="11" max="11" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.90625" customWidth="1"/>
+    <col min="14" max="14" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6328125" customWidth="1"/>
+    <col min="17" max="17" width="31.6328125" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:R2" si="0">COUNTA(C7:C10006)</f>
-        <v>87</v>
+        <f>COUNTA(C7:C10006)</f>
+        <v>96</v>
       </c>
       <c r="D2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(D7:D10006)</f>
+        <v>96</v>
       </c>
       <c r="E2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(E7:E10006)</f>
+        <v>96</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(F7:F10006)</f>
+        <v>96</v>
       </c>
       <c r="G2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(G7:G10006)</f>
+        <v>96</v>
       </c>
       <c r="H2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(H7:H10006)</f>
+        <v>96</v>
       </c>
       <c r="I2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(I7:I10006)</f>
+        <v>96</v>
       </c>
       <c r="J2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(J7:J10006)</f>
+        <v>96</v>
       </c>
       <c r="K2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(K7:K10006)</f>
+        <v>96</v>
       </c>
       <c r="L2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(L7:L10006)</f>
+        <v>96</v>
       </c>
       <c r="M2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(M7:M10006)</f>
+        <v>96</v>
       </c>
       <c r="N2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(N7:N10006)</f>
+        <v>96</v>
       </c>
       <c r="O2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(O7:O10006)</f>
+        <v>96</v>
       </c>
       <c r="P2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(P7:P10006)</f>
+        <v>96</v>
       </c>
       <c r="Q2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(Q7:Q10006)</f>
+        <v>96</v>
       </c>
       <c r="R2">
-        <f t="shared" si="0"/>
-        <v>87</v>
+        <f>COUNTA(R7:R10006)</f>
+        <v>96</v>
       </c>
       <c r="Z2" t="s">
         <v>1</v>
       </c>
       <c r="AA2">
-        <f>AVERAGE(W7:W10006)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+        <f>AVERAGE(W7:W10005)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="Z3" t="s">
         <v>2</v>
       </c>
       <c r="AA3">
         <f>MAX(C2:R2)</f>
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1319,20 +1398,20 @@
         <v>4</v>
       </c>
       <c r="AA4">
-        <f>SUM(X7:X10006)</f>
+        <f>SUM(X7:X10005)</f>
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="Z5" t="s">
         <v>5</v>
       </c>
       <c r="AA5">
-        <f>COUNTIF(W7:W10006,"&lt;100")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+        <f>COUNTIF(W7:W10005,"&lt;100")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -1394,12 +1473,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="C7" t="str">
-        <f>_xlfn.CONCAT(D7,"Ω ",E7,"% ",F7," ",G7,"w ",I7," ",J7,"ppm/°C ",R7)</f>
+        <f t="shared" ref="C7:C38" si="0">_xlfn.CONCAT(D7,"Ω ",E7,"% ",F7," ",G7,"w ",I7," ",J7,"ppm/°C ",R7)</f>
         <v>100Ω 1% 0603 0.1w Thick Film 100ppm/°C  </v>
       </c>
       <c r="D7">
@@ -1470,12 +1549,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="C8" t="str">
-        <f>_xlfn.CONCAT(D8,"Ω ",E8,"% ",F8," ",G8,"w ",I8," ",J8,"ppm/°C ",R8)</f>
+        <f t="shared" si="0"/>
         <v>470kΩ 1% 01005 0.03w Thick Film 200ppm/°C  </v>
       </c>
       <c r="D8" t="s">
@@ -1539,12 +1618,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3</v>
       </c>
       <c r="C9" t="str">
-        <f>_xlfn.CONCAT(D9,"Ω ",E9,"% ",F9," ",G9,"w ",I9," ",J9,"ppm/°C ",R9)</f>
+        <f t="shared" si="0"/>
         <v>1kΩ 1% 01005 0.03w Thick Film 200ppm/°C  </v>
       </c>
       <c r="D9" t="s">
@@ -1608,12 +1687,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>4</v>
       </c>
       <c r="C10" t="str">
-        <f>_xlfn.CONCAT(D10,"Ω ",E10,"% ",F10," ",G10,"w ",I10," ",J10,"ppm/°C ",R10)</f>
+        <f t="shared" si="0"/>
         <v>2.2kΩ 5% 01005 0.03w Thick Film 200ppm/°C  </v>
       </c>
       <c r="D10" t="s">
@@ -1677,12 +1756,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>5</v>
       </c>
       <c r="C11" t="str">
-        <f>_xlfn.CONCAT(D11,"Ω ",E11,"% ",F11," ",G11,"w ",I11," ",J11,"ppm/°C ",R11)</f>
+        <f t="shared" si="0"/>
         <v>1MΩ 1% 01005 0.03w Thick Film 200ppm/°C  </v>
       </c>
       <c r="D11" t="s">
@@ -1746,12 +1825,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="C12" t="str">
-        <f>_xlfn.CONCAT(D12,"Ω ",E12,"% ",F12," ",G12,"w ",I12," ",J12,"ppm/°C ",R12)</f>
+        <f t="shared" si="0"/>
         <v>0Ω  % 0603 0.1w Thick Film 200ppm/°C Automotive</v>
       </c>
       <c r="D12">
@@ -1815,12 +1894,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>7</v>
       </c>
       <c r="C13" t="str">
-        <f>_xlfn.CONCAT(D13,"Ω ",E13,"% ",F13," ",G13,"w ",I13," ",J13,"ppm/°C ",R13)</f>
+        <f t="shared" si="0"/>
         <v>0Ω  % 0805 0.125w Thick Film 200ppm/°C Automotive</v>
       </c>
       <c r="D13">
@@ -1884,12 +1963,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>8</v>
       </c>
       <c r="C14" t="str">
-        <f>_xlfn.CONCAT(D14,"Ω ",E14,"% ",F14," ",G14,"w ",I14," ",J14,"ppm/°C ",R14)</f>
+        <f t="shared" si="0"/>
         <v>0Ω  % 1206 0.25w Thick Film 200ppm/°C Automotive</v>
       </c>
       <c r="D14">
@@ -1953,12 +2032,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>9</v>
       </c>
       <c r="C15" t="str">
-        <f>_xlfn.CONCAT(D15,"Ω ",E15,"% ",F15," ",G15,"w ",I15," ",J15,"ppm/°C ",R15)</f>
+        <f t="shared" si="0"/>
         <v>22Ω 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D15">
@@ -2022,12 +2101,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>10</v>
       </c>
       <c r="C16" t="str">
-        <f>_xlfn.CONCAT(D16,"Ω ",E16,"% ",F16," ",G16,"w ",I16," ",J16,"ppm/°C ",R16)</f>
+        <f t="shared" si="0"/>
         <v>68Ω 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D16">
@@ -2091,12 +2170,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>11</v>
       </c>
       <c r="C17" t="str">
-        <f>_xlfn.CONCAT(D17,"Ω ",E17,"% ",F17," ",G17,"w ",I17," ",J17,"ppm/°C ",R17)</f>
+        <f t="shared" si="0"/>
         <v>75Ω 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D17">
@@ -2160,12 +2239,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>12</v>
       </c>
       <c r="C18" t="str">
-        <f>_xlfn.CONCAT(D18,"Ω ",E18,"% ",F18," ",G18,"w ",I18," ",J18,"ppm/°C ",R18)</f>
+        <f t="shared" si="0"/>
         <v>100Ω 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D18">
@@ -2229,12 +2308,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>13</v>
       </c>
       <c r="C19" t="str">
-        <f>_xlfn.CONCAT(D19,"Ω ",E19,"% ",F19," ",G19,"w ",I19," ",J19,"ppm/°C ",R19)</f>
+        <f t="shared" si="0"/>
         <v>220Ω 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D19">
@@ -2298,12 +2377,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>14</v>
       </c>
       <c r="C20" t="str">
-        <f>_xlfn.CONCAT(D20,"Ω ",E20,"% ",F20," ",G20,"w ",I20," ",J20,"ppm/°C ",R20)</f>
+        <f t="shared" si="0"/>
         <v>470Ω 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D20">
@@ -2367,12 +2446,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>15</v>
       </c>
       <c r="C21" t="str">
-        <f>_xlfn.CONCAT(D21,"Ω ",E21,"% ",F21," ",G21,"w ",I21," ",J21,"ppm/°C ",R21)</f>
+        <f t="shared" si="0"/>
         <v>560Ω 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D21">
@@ -2436,12 +2515,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>16</v>
       </c>
       <c r="C22" t="str">
-        <f>_xlfn.CONCAT(D22,"Ω ",E22,"% ",F22," ",G22,"w ",I22," ",J22,"ppm/°C ",R22)</f>
+        <f t="shared" si="0"/>
         <v>680Ω 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D22">
@@ -2505,12 +2584,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>17</v>
       </c>
       <c r="C23" t="str">
-        <f>_xlfn.CONCAT(D23,"Ω ",E23,"% ",F23," ",G23,"w ",I23," ",J23,"ppm/°C ",R23)</f>
+        <f t="shared" si="0"/>
         <v>750Ω 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D23">
@@ -2574,12 +2653,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>18</v>
       </c>
       <c r="C24" t="str">
-        <f>_xlfn.CONCAT(D24,"Ω ",E24,"% ",F24," ",G24,"w ",I24," ",J24,"ppm/°C ",R24)</f>
+        <f t="shared" si="0"/>
         <v>2.2kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D24" t="s">
@@ -2643,12 +2722,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>19</v>
       </c>
       <c r="C25" t="str">
-        <f>_xlfn.CONCAT(D25,"Ω ",E25,"% ",F25," ",G25,"w ",I25," ",J25,"ppm/°C ",R25)</f>
+        <f t="shared" si="0"/>
         <v>3.3kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D25" t="s">
@@ -2712,12 +2791,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>20</v>
       </c>
       <c r="C26" t="str">
-        <f>_xlfn.CONCAT(D26,"Ω ",E26,"% ",F26," ",G26,"w ",I26," ",J26,"ppm/°C ",R26)</f>
+        <f t="shared" si="0"/>
         <v>4.7kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D26" t="s">
@@ -2781,12 +2860,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>21</v>
       </c>
       <c r="C27" t="str">
-        <f>_xlfn.CONCAT(D27,"Ω ",E27,"% ",F27," ",G27,"w ",I27," ",J27,"ppm/°C ",R27)</f>
+        <f t="shared" si="0"/>
         <v>5.6kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D27" t="s">
@@ -2850,12 +2929,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>22</v>
       </c>
       <c r="C28" t="str">
-        <f>_xlfn.CONCAT(D28,"Ω ",E28,"% ",F28," ",G28,"w ",I28," ",J28,"ppm/°C ",R28)</f>
+        <f t="shared" si="0"/>
         <v>6.8kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D28" t="s">
@@ -2919,12 +2998,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>23</v>
       </c>
       <c r="C29" t="str">
-        <f>_xlfn.CONCAT(D29,"Ω ",E29,"% ",F29," ",G29,"w ",I29," ",J29,"ppm/°C ",R29)</f>
+        <f t="shared" si="0"/>
         <v>7.5kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D29" t="s">
@@ -2988,12 +3067,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>24</v>
       </c>
       <c r="C30" t="str">
-        <f>_xlfn.CONCAT(D30,"Ω ",E30,"% ",F30," ",G30,"w ",I30," ",J30,"ppm/°C ",R30)</f>
+        <f t="shared" si="0"/>
         <v>22kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D30" t="s">
@@ -3057,12 +3136,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>25</v>
       </c>
       <c r="C31" t="str">
-        <f>_xlfn.CONCAT(D31,"Ω ",E31,"% ",F31," ",G31,"w ",I31," ",J31,"ppm/°C ",R31)</f>
+        <f t="shared" si="0"/>
         <v>33kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D31" t="s">
@@ -3126,12 +3205,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>26</v>
       </c>
       <c r="C32" t="str">
-        <f>_xlfn.CONCAT(D32,"Ω ",E32,"% ",F32," ",G32,"w ",I32," ",J32,"ppm/°C ",R32)</f>
+        <f t="shared" si="0"/>
         <v>47kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D32" t="s">
@@ -3195,12 +3274,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>27</v>
       </c>
       <c r="C33" t="str">
-        <f>_xlfn.CONCAT(D33,"Ω ",E33,"% ",F33," ",G33,"w ",I33," ",J33,"ppm/°C ",R33)</f>
+        <f t="shared" si="0"/>
         <v>56kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D33" t="s">
@@ -3264,12 +3343,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>28</v>
       </c>
       <c r="C34" t="str">
-        <f>_xlfn.CONCAT(D34,"Ω ",E34,"% ",F34," ",G34,"w ",I34," ",J34,"ppm/°C ",R34)</f>
+        <f t="shared" si="0"/>
         <v>68kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D34" t="s">
@@ -3333,12 +3412,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>29</v>
       </c>
       <c r="C35" t="str">
-        <f>_xlfn.CONCAT(D35,"Ω ",E35,"% ",F35," ",G35,"w ",I35," ",J35,"ppm/°C ",R35)</f>
+        <f t="shared" si="0"/>
         <v>75kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D35" t="s">
@@ -3402,12 +3481,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>30</v>
       </c>
       <c r="C36" t="str">
-        <f>_xlfn.CONCAT(D36,"Ω ",E36,"% ",F36," ",G36,"w ",I36," ",J36,"ppm/°C ",R36)</f>
+        <f t="shared" si="0"/>
         <v>100kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D36" t="s">
@@ -3471,12 +3550,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>31</v>
       </c>
       <c r="C37" t="str">
-        <f>_xlfn.CONCAT(D37,"Ω ",E37,"% ",F37," ",G37,"w ",I37," ",J37,"ppm/°C ",R37)</f>
+        <f t="shared" si="0"/>
         <v>5.1kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D37" t="s">
@@ -3540,12 +3619,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>32</v>
       </c>
       <c r="C38" t="str">
-        <f>_xlfn.CONCAT(D38,"Ω ",E38,"% ",F38," ",G38,"w ",I38," ",J38,"ppm/°C ",R38)</f>
+        <f t="shared" si="0"/>
         <v>22Ω 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D38">
@@ -3609,12 +3688,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>33</v>
       </c>
       <c r="C39" t="str">
-        <f>_xlfn.CONCAT(D39,"Ω ",E39,"% ",F39," ",G39,"w ",I39," ",J39,"ppm/°C ",R39)</f>
+        <f t="shared" ref="C39:C70" si="10">_xlfn.CONCAT(D39,"Ω ",E39,"% ",F39," ",G39,"w ",I39," ",J39,"ppm/°C ",R39)</f>
         <v>68Ω 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D39">
@@ -3678,12 +3757,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>34</v>
       </c>
       <c r="C40" t="str">
-        <f>_xlfn.CONCAT(D40,"Ω ",E40,"% ",F40," ",G40,"w ",I40," ",J40,"ppm/°C ",R40)</f>
+        <f t="shared" si="10"/>
         <v>75Ω 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D40">
@@ -3747,12 +3826,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>35</v>
       </c>
       <c r="C41" t="str">
-        <f>_xlfn.CONCAT(D41,"Ω ",E41,"% ",F41," ",G41,"w ",I41," ",J41,"ppm/°C ",R41)</f>
+        <f t="shared" si="10"/>
         <v>100Ω 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D41">
@@ -3816,12 +3895,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>36</v>
       </c>
       <c r="C42" t="str">
-        <f>_xlfn.CONCAT(D42,"Ω ",E42,"% ",F42," ",G42,"w ",I42," ",J42,"ppm/°C ",R42)</f>
+        <f t="shared" si="10"/>
         <v>220Ω 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D42">
@@ -3885,12 +3964,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>37</v>
       </c>
       <c r="C43" t="str">
-        <f>_xlfn.CONCAT(D43,"Ω ",E43,"% ",F43," ",G43,"w ",I43," ",J43,"ppm/°C ",R43)</f>
+        <f t="shared" si="10"/>
         <v>330Ω 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D43">
@@ -3954,12 +4033,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>38</v>
       </c>
       <c r="C44" t="str">
-        <f>_xlfn.CONCAT(D44,"Ω ",E44,"% ",F44," ",G44,"w ",I44," ",J44,"ppm/°C ",R44)</f>
+        <f t="shared" si="10"/>
         <v>470Ω 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D44">
@@ -4023,12 +4102,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>39</v>
       </c>
       <c r="C45" t="str">
-        <f>_xlfn.CONCAT(D45,"Ω ",E45,"% ",F45," ",G45,"w ",I45," ",J45,"ppm/°C ",R45)</f>
+        <f t="shared" si="10"/>
         <v>560Ω 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D45">
@@ -4092,12 +4171,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>40</v>
       </c>
       <c r="C46" t="str">
-        <f>_xlfn.CONCAT(D46,"Ω ",E46,"% ",F46," ",G46,"w ",I46," ",J46,"ppm/°C ",R46)</f>
+        <f t="shared" si="10"/>
         <v>680Ω 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D46">
@@ -4161,12 +4240,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>41</v>
       </c>
       <c r="C47" t="str">
-        <f>_xlfn.CONCAT(D47,"Ω ",E47,"% ",F47," ",G47,"w ",I47," ",J47,"ppm/°C ",R47)</f>
+        <f t="shared" si="10"/>
         <v>750Ω 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D47">
@@ -4230,13 +4309,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>42</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" t="str">
-        <f>_xlfn.CONCAT(D48,"Ω ",E48,"% ",F48," ",G48,"w ",I48," ",J48,"ppm/°C ",R48)</f>
+        <f t="shared" si="10"/>
         <v>1kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D48" t="s">
@@ -4300,12 +4379,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>43</v>
       </c>
       <c r="C49" t="str">
-        <f>_xlfn.CONCAT(D49,"Ω ",E49,"% ",F49," ",G49,"w ",I49," ",J49,"ppm/°C ",R49)</f>
+        <f t="shared" si="10"/>
         <v>2.2kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D49" t="s">
@@ -4369,12 +4448,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>44</v>
       </c>
       <c r="C50" t="str">
-        <f>_xlfn.CONCAT(D50,"Ω ",E50,"% ",F50," ",G50,"w ",I50," ",J50,"ppm/°C ",R50)</f>
+        <f t="shared" si="10"/>
         <v>3.3kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D50" t="s">
@@ -4438,12 +4517,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>45</v>
       </c>
       <c r="C51" t="str">
-        <f>_xlfn.CONCAT(D51,"Ω ",E51,"% ",F51," ",G51,"w ",I51," ",J51,"ppm/°C ",R51)</f>
+        <f t="shared" si="10"/>
         <v>4.7kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D51" t="s">
@@ -4507,12 +4586,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>46</v>
       </c>
       <c r="C52" t="str">
-        <f>_xlfn.CONCAT(D52,"Ω ",E52,"% ",F52," ",G52,"w ",I52," ",J52,"ppm/°C ",R52)</f>
+        <f t="shared" si="10"/>
         <v>5.6kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D52" t="s">
@@ -4576,12 +4655,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>47</v>
       </c>
       <c r="C53" t="str">
-        <f>_xlfn.CONCAT(D53,"Ω ",E53,"% ",F53," ",G53,"w ",I53," ",J53,"ppm/°C ",R53)</f>
+        <f t="shared" si="10"/>
         <v>6.8kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D53" t="s">
@@ -4645,12 +4724,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>48</v>
       </c>
       <c r="C54" t="str">
-        <f>_xlfn.CONCAT(D54,"Ω ",E54,"% ",F54," ",G54,"w ",I54," ",J54,"ppm/°C ",R54)</f>
+        <f t="shared" si="10"/>
         <v>7.5kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D54" t="s">
@@ -4714,12 +4793,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>49</v>
       </c>
       <c r="C55" t="str">
-        <f>_xlfn.CONCAT(D55,"Ω ",E55,"% ",F55," ",G55,"w ",I55," ",J55,"ppm/°C ",R55)</f>
+        <f t="shared" si="10"/>
         <v>10kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D55" t="s">
@@ -4783,12 +4862,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>50</v>
       </c>
       <c r="C56" t="str">
-        <f>_xlfn.CONCAT(D56,"Ω ",E56,"% ",F56," ",G56,"w ",I56," ",J56,"ppm/°C ",R56)</f>
+        <f t="shared" si="10"/>
         <v>22kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D56" t="s">
@@ -4852,12 +4931,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>51</v>
       </c>
       <c r="C57" t="str">
-        <f>_xlfn.CONCAT(D57,"Ω ",E57,"% ",F57," ",G57,"w ",I57," ",J57,"ppm/°C ",R57)</f>
+        <f t="shared" si="10"/>
         <v>33kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D57" t="s">
@@ -4921,12 +5000,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>52</v>
       </c>
       <c r="C58" t="str">
-        <f>_xlfn.CONCAT(D58,"Ω ",E58,"% ",F58," ",G58,"w ",I58," ",J58,"ppm/°C ",R58)</f>
+        <f t="shared" si="10"/>
         <v>47kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D58" t="s">
@@ -4990,12 +5069,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>53</v>
       </c>
       <c r="C59" t="str">
-        <f>_xlfn.CONCAT(D59,"Ω ",E59,"% ",F59," ",G59,"w ",I59," ",J59,"ppm/°C ",R59)</f>
+        <f t="shared" si="10"/>
         <v>56kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D59" t="s">
@@ -5059,12 +5138,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>54</v>
       </c>
       <c r="C60" t="str">
-        <f>_xlfn.CONCAT(D60,"Ω ",E60,"% ",F60," ",G60,"w ",I60," ",J60,"ppm/°C ",R60)</f>
+        <f t="shared" si="10"/>
         <v>68kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D60" t="s">
@@ -5128,12 +5207,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>55</v>
       </c>
       <c r="C61" t="str">
-        <f>_xlfn.CONCAT(D61,"Ω ",E61,"% ",F61," ",G61,"w ",I61," ",J61,"ppm/°C ",R61)</f>
+        <f t="shared" si="10"/>
         <v>75kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D61" t="s">
@@ -5197,12 +5276,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>56</v>
       </c>
       <c r="C62" t="str">
-        <f>_xlfn.CONCAT(D62,"Ω ",E62,"% ",F62," ",G62,"w ",I62," ",J62,"ppm/°C ",R62)</f>
+        <f t="shared" si="10"/>
         <v>100kΩ 1% 0805 0.125w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D62" t="s">
@@ -5266,12 +5345,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>57</v>
       </c>
       <c r="C63" t="str">
-        <f>_xlfn.CONCAT(D63,"Ω ",E63,"% ",F63," ",G63,"w ",I63," ",J63,"ppm/°C ",R63)</f>
+        <f t="shared" si="10"/>
         <v>22Ω 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D63">
@@ -5335,12 +5414,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>58</v>
       </c>
       <c r="C64" t="str">
-        <f>_xlfn.CONCAT(D64,"Ω ",E64,"% ",F64," ",G64,"w ",I64," ",J64,"ppm/°C ",R64)</f>
+        <f t="shared" si="10"/>
         <v>68Ω 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D64">
@@ -5404,12 +5483,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>59</v>
       </c>
       <c r="C65" t="str">
-        <f>_xlfn.CONCAT(D65,"Ω ",E65,"% ",F65," ",G65,"w ",I65," ",J65,"ppm/°C ",R65)</f>
+        <f t="shared" si="10"/>
         <v>75Ω 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D65">
@@ -5473,12 +5552,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>60</v>
       </c>
       <c r="C66" t="str">
-        <f>_xlfn.CONCAT(D66,"Ω ",E66,"% ",F66," ",G66,"w ",I66," ",J66,"ppm/°C ",R66)</f>
+        <f t="shared" si="10"/>
         <v>100Ω 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D66">
@@ -5542,12 +5621,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>61</v>
       </c>
       <c r="C67" t="str">
-        <f>_xlfn.CONCAT(D67,"Ω ",E67,"% ",F67," ",G67,"w ",I67," ",J67,"ppm/°C ",R67)</f>
+        <f t="shared" si="10"/>
         <v>220Ω 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D67">
@@ -5611,12 +5690,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>62</v>
       </c>
       <c r="C68" t="str">
-        <f>_xlfn.CONCAT(D68,"Ω ",E68,"% ",F68," ",G68,"w ",I68," ",J68,"ppm/°C ",R68)</f>
+        <f t="shared" si="10"/>
         <v>330Ω 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D68">
@@ -5680,12 +5759,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>63</v>
       </c>
       <c r="C69" t="str">
-        <f>_xlfn.CONCAT(D69,"Ω ",E69,"% ",F69," ",G69,"w ",I69," ",J69,"ppm/°C ",R69)</f>
+        <f t="shared" si="10"/>
         <v>470Ω 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D69">
@@ -5749,12 +5828,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>64</v>
       </c>
       <c r="C70" t="str">
-        <f>_xlfn.CONCAT(D70,"Ω ",E70,"% ",F70," ",G70,"w ",I70," ",J70,"ppm/°C ",R70)</f>
+        <f t="shared" si="10"/>
         <v>560Ω 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D70">
@@ -5818,12 +5897,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>65</v>
       </c>
       <c r="C71" t="str">
-        <f>_xlfn.CONCAT(D71,"Ω ",E71,"% ",F71," ",G71,"w ",I71," ",J71,"ppm/°C ",R71)</f>
+        <f t="shared" ref="C71:C93" si="11">_xlfn.CONCAT(D71,"Ω ",E71,"% ",F71," ",G71,"w ",I71," ",J71,"ppm/°C ",R71)</f>
         <v>680Ω 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D71">
@@ -5887,12 +5966,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>66</v>
       </c>
       <c r="C72" t="str">
-        <f>_xlfn.CONCAT(D72,"Ω ",E72,"% ",F72," ",G72,"w ",I72," ",J72,"ppm/°C ",R72)</f>
+        <f t="shared" si="11"/>
         <v>750Ω 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D72">
@@ -5956,12 +6035,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>67</v>
       </c>
       <c r="C73" t="str">
-        <f>_xlfn.CONCAT(D73,"Ω ",E73,"% ",F73," ",G73,"w ",I73," ",J73,"ppm/°C ",R73)</f>
+        <f t="shared" si="11"/>
         <v>2.2kΩ 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D73" t="s">
@@ -6025,12 +6104,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>68</v>
       </c>
       <c r="C74" t="str">
-        <f>_xlfn.CONCAT(D74,"Ω ",E74,"% ",F74," ",G74,"w ",I74," ",J74,"ppm/°C ",R74)</f>
+        <f t="shared" si="11"/>
         <v>3.3kΩ 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D74" t="s">
@@ -6094,12 +6173,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>69</v>
       </c>
       <c r="C75" t="str">
-        <f>_xlfn.CONCAT(D75,"Ω ",E75,"% ",F75," ",G75,"w ",I75," ",J75,"ppm/°C ",R75)</f>
+        <f t="shared" si="11"/>
         <v>5.6kΩ 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D75" t="s">
@@ -6163,12 +6242,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>70</v>
       </c>
       <c r="C76" t="str">
-        <f>_xlfn.CONCAT(D76,"Ω ",E76,"% ",F76," ",G76,"w ",I76," ",J76,"ppm/°C ",R76)</f>
+        <f t="shared" si="11"/>
         <v>6.8kΩ 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D76" t="s">
@@ -6232,12 +6311,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>71</v>
       </c>
       <c r="C77" t="str">
-        <f>_xlfn.CONCAT(D77,"Ω ",E77,"% ",F77," ",G77,"w ",I77," ",J77,"ppm/°C ",R77)</f>
+        <f t="shared" si="11"/>
         <v>7.5kΩ 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D77" t="s">
@@ -6301,12 +6380,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>72</v>
       </c>
       <c r="C78" t="str">
-        <f>_xlfn.CONCAT(D78,"Ω ",E78,"% ",F78," ",G78,"w ",I78," ",J78,"ppm/°C ",R78)</f>
+        <f t="shared" si="11"/>
         <v>22kΩ 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D78" t="s">
@@ -6370,12 +6449,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>73</v>
       </c>
       <c r="C79" t="str">
-        <f>_xlfn.CONCAT(D79,"Ω ",E79,"% ",F79," ",G79,"w ",I79," ",J79,"ppm/°C ",R79)</f>
+        <f t="shared" si="11"/>
         <v>33kΩ 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D79" t="s">
@@ -6439,12 +6518,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>74</v>
       </c>
       <c r="C80" t="str">
-        <f>_xlfn.CONCAT(D80,"Ω ",E80,"% ",F80," ",G80,"w ",I80," ",J80,"ppm/°C ",R80)</f>
+        <f t="shared" si="11"/>
         <v>47kΩ 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D80" t="s">
@@ -6508,12 +6587,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>75</v>
       </c>
       <c r="C81" t="str">
-        <f>_xlfn.CONCAT(D81,"Ω ",E81,"% ",F81," ",G81,"w ",I81," ",J81,"ppm/°C ",R81)</f>
+        <f t="shared" si="11"/>
         <v>56kΩ 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D81" t="s">
@@ -6577,12 +6656,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>76</v>
       </c>
       <c r="C82" t="str">
-        <f>_xlfn.CONCAT(D82,"Ω ",E82,"% ",F82," ",G82,"w ",I82," ",J82,"ppm/°C ",R82)</f>
+        <f t="shared" si="11"/>
         <v>68kΩ 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D82" t="s">
@@ -6646,12 +6725,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>77</v>
       </c>
       <c r="C83" t="str">
-        <f>_xlfn.CONCAT(D83,"Ω ",E83,"% ",F83," ",G83,"w ",I83," ",J83,"ppm/°C ",R83)</f>
+        <f t="shared" si="11"/>
         <v>75kΩ 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D83" t="s">
@@ -6715,12 +6794,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>78</v>
       </c>
       <c r="C84" t="str">
-        <f>_xlfn.CONCAT(D84,"Ω ",E84,"% ",F84," ",G84,"w ",I84," ",J84,"ppm/°C ",R84)</f>
+        <f t="shared" si="11"/>
         <v>330Ω 5% 1206 0.25w Thick Film 200ppm/°C Automotive</v>
       </c>
       <c r="D84">
@@ -6784,12 +6863,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>79</v>
       </c>
       <c r="C85" t="str">
-        <f>_xlfn.CONCAT(D85,"Ω ",E85,"% ",F85," ",G85,"w ",I85," ",J85,"ppm/°C ",R85)</f>
+        <f t="shared" si="11"/>
         <v>10kΩ 1% 1206 0.25w Thick Film 200ppm/°C Automotive</v>
       </c>
       <c r="D85" t="s">
@@ -6841,24 +6920,24 @@
         <v>1</v>
       </c>
       <c r="V85">
-        <f t="shared" ref="V85:V93" si="10">COUNTBLANK(C85:R85)</f>
+        <f t="shared" ref="V85:V93" si="12">COUNTBLANK(C85:R85)</f>
         <v>0</v>
       </c>
       <c r="W85">
-        <f t="shared" ref="W85:W93" si="11">100*COUNTA(C85:R85)/$AA$7</f>
+        <f t="shared" ref="W85:W93" si="13">100*COUNTA(C85:R85)/$AA$7</f>
         <v>100</v>
       </c>
       <c r="X85">
-        <f t="shared" ref="X85:X93" si="12">IF(W85=100,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
+        <f t="shared" ref="X85:X93" si="14">IF(W85=100,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>80</v>
       </c>
       <c r="C86" t="str">
-        <f>_xlfn.CONCAT(D86,"Ω ",E86,"% ",F86," ",G86,"w ",I86," ",J86,"ppm/°C ",R86)</f>
+        <f t="shared" si="11"/>
         <v>470Ω 5% 1206 0.25w Thick Film 200ppm/°C Automotive</v>
       </c>
       <c r="D86">
@@ -6910,24 +6989,24 @@
         <v>1</v>
       </c>
       <c r="V86">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W86">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="X86">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>81</v>
       </c>
       <c r="C87" t="str">
-        <f>_xlfn.CONCAT(D87,"Ω ",E87,"% ",F87," ",G87,"w ",I87," ",J87,"ppm/°C ",R87)</f>
+        <f t="shared" si="11"/>
         <v>4.7kΩ 1% 1206 0.25w Thick Film 200ppm/°C Automotive</v>
       </c>
       <c r="D87" t="s">
@@ -6979,24 +7058,24 @@
         <v>1</v>
       </c>
       <c r="V87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W87">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="X87">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>82</v>
       </c>
       <c r="C88" t="str">
-        <f>_xlfn.CONCAT(D88,"Ω ",E88,"% ",F88," ",G88,"w ",I88," ",J88,"ppm/°C ",R88)</f>
+        <f t="shared" si="11"/>
         <v>100kΩ 1% 1206 0.25w Thick Film 200ppm/°C Automotive</v>
       </c>
       <c r="D88" t="s">
@@ -7048,24 +7127,24 @@
         <v>1</v>
       </c>
       <c r="V88">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W88">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="X88">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>83</v>
       </c>
       <c r="C89" t="str">
-        <f>_xlfn.CONCAT(D89,"Ω ",E89,"% ",F89," ",G89,"w ",I89," ",J89,"ppm/°C ",R89)</f>
+        <f t="shared" si="11"/>
         <v>1kΩ 1% 1206 0.25w Thick Film 200ppm/°C Automotive</v>
       </c>
       <c r="D89" t="s">
@@ -7117,24 +7196,24 @@
         <v>1</v>
       </c>
       <c r="V89">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W89">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="X89">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>84</v>
       </c>
       <c r="C90" t="str">
-        <f>_xlfn.CONCAT(D90,"Ω ",E90,"% ",F90," ",G90,"w ",I90," ",J90,"ppm/°C ",R90)</f>
+        <f t="shared" si="11"/>
         <v>220Ω 5% 1206 0.25w Thick Film 200ppm/°C Automotive</v>
       </c>
       <c r="D90">
@@ -7186,24 +7265,24 @@
         <v>1</v>
       </c>
       <c r="V90">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W90">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="X90">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>85</v>
       </c>
       <c r="C91" t="str">
-        <f>_xlfn.CONCAT(D91,"Ω ",E91,"% ",F91," ",G91,"w ",I91," ",J91,"ppm/°C ",R91)</f>
+        <f t="shared" si="11"/>
         <v>330Ω 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D91">
@@ -7255,24 +7334,24 @@
         <v>1</v>
       </c>
       <c r="V91">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W91">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="X91">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>86</v>
       </c>
       <c r="C92" t="str">
-        <f>_xlfn.CONCAT(D92,"Ω ",E92,"% ",F92," ",G92,"w ",I92," ",J92,"ppm/°C ",R92)</f>
+        <f t="shared" si="11"/>
         <v>1kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D92" t="s">
@@ -7324,24 +7403,24 @@
         <v>1</v>
       </c>
       <c r="V92">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W92">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="X92">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>87</v>
       </c>
       <c r="C93" t="str">
-        <f>_xlfn.CONCAT(D93,"Ω ",E93,"% ",F93," ",G93,"w ",I93," ",J93,"ppm/°C ",R93)</f>
+        <f t="shared" si="11"/>
         <v>10kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
       </c>
       <c r="D93" t="s">
@@ -7393,26 +7472,545 @@
         <v>1</v>
       </c>
       <c r="V93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W93">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="X93">
-        <f t="shared" si="12"/>
-        <v>1</v>
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>88</v>
+      </c>
+      <c r="C94" t="str">
+        <f>_xlfn.CONCAT(D94,"Ω ",E94,"% ",F94," ",G94,"w ",I94," ",J94,"ppm/°C ",R94)</f>
+        <v>10kΩ 0.1% 0603 0.1w Thin Film 25ppm/°C Automotive</v>
+      </c>
+      <c r="D94" t="s">
+        <v>45</v>
+      </c>
+      <c r="E94">
+        <v>0.1</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G94">
+        <v>0.1</v>
+      </c>
+      <c r="H94" t="s">
+        <v>27</v>
+      </c>
+      <c r="I94" t="s">
+        <v>246</v>
+      </c>
+      <c r="J94">
+        <v>25</v>
+      </c>
+      <c r="K94" t="s">
+        <v>245</v>
+      </c>
+      <c r="L94" t="s">
+        <v>243</v>
+      </c>
+      <c r="M94" t="s">
+        <v>31</v>
+      </c>
+      <c r="N94" t="s">
+        <v>244</v>
+      </c>
+      <c r="O94" t="s">
+        <v>247</v>
+      </c>
+      <c r="P94" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>35</v>
+      </c>
+      <c r="R94" t="s">
+        <v>44</v>
+      </c>
+      <c r="S94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>89</v>
+      </c>
+      <c r="C95" t="str">
+        <f>_xlfn.CONCAT(D95,"Ω ",E95,"% ",F95," ",G95,"w ",I95," ",J95,"ppm/°C ",R95)</f>
+        <v>10kΩ 0.1% 0805 0.125w Thin Film 25ppm/°C Automotive</v>
+      </c>
+      <c r="D95" t="s">
+        <v>45</v>
+      </c>
+      <c r="E95">
+        <v>0.1</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G95">
+        <v>0.125</v>
+      </c>
+      <c r="H95" t="s">
+        <v>252</v>
+      </c>
+      <c r="I95" t="s">
+        <v>246</v>
+      </c>
+      <c r="J95">
+        <v>25</v>
+      </c>
+      <c r="K95" t="s">
+        <v>245</v>
+      </c>
+      <c r="L95" t="s">
+        <v>248</v>
+      </c>
+      <c r="M95" t="s">
+        <v>31</v>
+      </c>
+      <c r="N95" t="s">
+        <v>249</v>
+      </c>
+      <c r="O95" t="s">
+        <v>247</v>
+      </c>
+      <c r="P95" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>86</v>
+      </c>
+      <c r="R95" t="s">
+        <v>44</v>
+      </c>
+      <c r="S95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>90</v>
+      </c>
+      <c r="C96" t="str">
+        <f>_xlfn.CONCAT(D96,"Ω ",E96,"% ",F96," ",G96,"w ",I96," ",J96,"ppm/°C ",R96)</f>
+        <v>10kΩ 0.1% 1206 0.25w Thin Film 25ppm/°C Automotive</v>
+      </c>
+      <c r="D96" t="s">
+        <v>45</v>
+      </c>
+      <c r="E96">
+        <v>0.1</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G96">
+        <v>0.25</v>
+      </c>
+      <c r="H96" t="s">
+        <v>81</v>
+      </c>
+      <c r="I96" t="s">
+        <v>246</v>
+      </c>
+      <c r="J96">
+        <v>25</v>
+      </c>
+      <c r="K96" t="s">
+        <v>245</v>
+      </c>
+      <c r="L96" t="s">
+        <v>250</v>
+      </c>
+      <c r="M96" t="s">
+        <v>31</v>
+      </c>
+      <c r="N96" t="s">
+        <v>251</v>
+      </c>
+      <c r="O96" t="s">
+        <v>247</v>
+      </c>
+      <c r="P96" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>43</v>
+      </c>
+      <c r="R96" t="s">
+        <v>44</v>
+      </c>
+      <c r="S96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>91</v>
+      </c>
+      <c r="C97" t="str">
+        <f>_xlfn.CONCAT(D97,"Ω ",E97,"% ",F97," ",G97,"w ",I97," ",J97,"ppm/°C ",R97)</f>
+        <v>110kΩ 0.1% 0603 0.1w Thin Film 25ppm/°C Automotive</v>
+      </c>
+      <c r="D97" t="s">
+        <v>253</v>
+      </c>
+      <c r="E97">
+        <v>0.1</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G97">
+        <v>0.1</v>
+      </c>
+      <c r="H97" t="s">
+        <v>27</v>
+      </c>
+      <c r="I97" t="s">
+        <v>246</v>
+      </c>
+      <c r="J97">
+        <v>25</v>
+      </c>
+      <c r="K97" t="s">
+        <v>245</v>
+      </c>
+      <c r="L97" t="s">
+        <v>254</v>
+      </c>
+      <c r="M97" t="s">
+        <v>31</v>
+      </c>
+      <c r="N97" t="s">
+        <v>255</v>
+      </c>
+      <c r="O97" t="s">
+        <v>247</v>
+      </c>
+      <c r="P97" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>35</v>
+      </c>
+      <c r="R97" t="s">
+        <v>44</v>
+      </c>
+      <c r="S97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>92</v>
+      </c>
+      <c r="C98" t="str">
+        <f>_xlfn.CONCAT(D98,"Ω ",E98,"% ",F98," ",G98,"w ",I98," ",J98,"ppm/°C ",R98)</f>
+        <v>110kΩ 0.1% 0805 0.125w Thin Film 25ppm/°C Automotive</v>
+      </c>
+      <c r="D98" t="s">
+        <v>253</v>
+      </c>
+      <c r="E98">
+        <v>0.1</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G98">
+        <v>0.125</v>
+      </c>
+      <c r="H98" t="s">
+        <v>252</v>
+      </c>
+      <c r="I98" t="s">
+        <v>246</v>
+      </c>
+      <c r="J98">
+        <v>25</v>
+      </c>
+      <c r="K98" t="s">
+        <v>245</v>
+      </c>
+      <c r="L98" t="s">
+        <v>256</v>
+      </c>
+      <c r="M98" t="s">
+        <v>31</v>
+      </c>
+      <c r="N98" t="s">
+        <v>257</v>
+      </c>
+      <c r="O98" t="s">
+        <v>247</v>
+      </c>
+      <c r="P98" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>86</v>
+      </c>
+      <c r="R98" t="s">
+        <v>44</v>
+      </c>
+      <c r="S98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>93</v>
+      </c>
+      <c r="C99" t="str">
+        <f>_xlfn.CONCAT(D99,"Ω ",E99,"% ",F99," ",G99,"w ",I99," ",J99,"ppm/°C ",R99)</f>
+        <v>110kΩ 0.1% 1206 0.25w Thin Film 25ppm/°C Automotive</v>
+      </c>
+      <c r="D99" t="s">
+        <v>253</v>
+      </c>
+      <c r="E99">
+        <v>0.1</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G99">
+        <v>0.25</v>
+      </c>
+      <c r="H99" t="s">
+        <v>81</v>
+      </c>
+      <c r="I99" t="s">
+        <v>246</v>
+      </c>
+      <c r="J99">
+        <v>25</v>
+      </c>
+      <c r="K99" t="s">
+        <v>245</v>
+      </c>
+      <c r="L99" t="s">
+        <v>258</v>
+      </c>
+      <c r="M99" t="s">
+        <v>31</v>
+      </c>
+      <c r="N99" t="s">
+        <v>259</v>
+      </c>
+      <c r="O99" t="s">
+        <v>247</v>
+      </c>
+      <c r="P99" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>43</v>
+      </c>
+      <c r="R99" t="s">
+        <v>44</v>
+      </c>
+      <c r="S99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>94</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" ref="C100:C102" si="15">_xlfn.CONCAT(D100,"Ω ",E100,"% ",F100," ",G100,"w ",I100," ",J100,"ppm/°C ",R100)</f>
+        <v>110kΩ 1% 0603 0.1w Thick Film 100ppm/°C Automotive</v>
+      </c>
+      <c r="D100" t="s">
+        <v>253</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G100">
+        <v>0.1</v>
+      </c>
+      <c r="H100" t="s">
+        <v>27</v>
+      </c>
+      <c r="I100" t="s">
+        <v>28</v>
+      </c>
+      <c r="J100">
+        <v>100</v>
+      </c>
+      <c r="K100" t="s">
+        <v>29</v>
+      </c>
+      <c r="L100" t="s">
+        <v>260</v>
+      </c>
+      <c r="M100" t="s">
+        <v>31</v>
+      </c>
+      <c r="N100" t="s">
+        <v>261</v>
+      </c>
+      <c r="O100" t="s">
+        <v>262</v>
+      </c>
+      <c r="P100" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>35</v>
+      </c>
+      <c r="R100" t="s">
+        <v>44</v>
+      </c>
+      <c r="S100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>95</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="15"/>
+        <v>110kΩ 1% 0805 0.125w Thick Film 100ppm/°C  </v>
+      </c>
+      <c r="D101" t="s">
+        <v>253</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G101">
+        <v>0.125</v>
+      </c>
+      <c r="H101" t="s">
+        <v>81</v>
+      </c>
+      <c r="I101" t="s">
+        <v>28</v>
+      </c>
+      <c r="J101">
+        <v>100</v>
+      </c>
+      <c r="K101" t="s">
+        <v>29</v>
+      </c>
+      <c r="L101" t="s">
+        <v>263</v>
+      </c>
+      <c r="M101" t="s">
+        <v>31</v>
+      </c>
+      <c r="N101" t="s">
+        <v>264</v>
+      </c>
+      <c r="O101" t="s">
+        <v>33</v>
+      </c>
+      <c r="P101" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>86</v>
+      </c>
+      <c r="R101" t="s">
+        <v>36</v>
+      </c>
+      <c r="S101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>96</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="15"/>
+        <v>110kΩ 1% 1206 0.25w Thick Film 100ppm/°C Automotive</v>
+      </c>
+      <c r="D102" t="s">
+        <v>253</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G102">
+        <v>0.25</v>
+      </c>
+      <c r="H102" t="s">
+        <v>38</v>
+      </c>
+      <c r="I102" t="s">
+        <v>28</v>
+      </c>
+      <c r="J102">
+        <v>100</v>
+      </c>
+      <c r="K102" t="s">
+        <v>29</v>
+      </c>
+      <c r="L102" t="s">
+        <v>265</v>
+      </c>
+      <c r="M102" t="s">
+        <v>31</v>
+      </c>
+      <c r="N102" t="s">
+        <v>266</v>
+      </c>
+      <c r="O102" t="s">
+        <v>262</v>
+      </c>
+      <c r="P102" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>43</v>
+      </c>
+      <c r="R102" t="s">
+        <v>44</v>
+      </c>
+      <c r="S102" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="C7:S253">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(C7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="L7:L253">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>